<commit_message>
remove pop up error when missing csv statistic file
</commit_message>
<xml_diff>
--- a/upload_data_with_monetization.xlsx
+++ b/upload_data_with_monetization.xlsx
@@ -466,12 +466,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>crige as fuck</t>
+          <t>sadasd</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>sdadsda</t>
+          <t>sdasd</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -481,7 +481,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>14:49</t>
+          <t>12:10</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
@@ -494,22 +494,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>crige as fuck</t>
+          <t>sadasd</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>sdadsda</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>10/24/2025</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>14:49</t>
+          <t>sdasd</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>

</xml_diff>